<commit_message>
added non pcb items to bom
</commit_message>
<xml_diff>
--- a/hardware/ACme++/rev_a/ACme++_bom.xlsx
+++ b/hardware/ACme++/rev_a/ACme++_bom.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="digikey_order.txt" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ACme" localSheetId="0">Sheet1!#REF!</definedName>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="266">
   <si>
     <t>Qty</t>
   </si>
@@ -797,6 +798,87 @@
   </si>
   <si>
     <t>0402-CAP</t>
+  </si>
+  <si>
+    <t>377-1709-ND</t>
+  </si>
+  <si>
+    <t>PPB-11860-BK</t>
+  </si>
+  <si>
+    <t>BOX ABS 3.09X2.09X1.65" BLK</t>
+  </si>
+  <si>
+    <t>377-1710-ND</t>
+  </si>
+  <si>
+    <t>PPB-11860-WT</t>
+  </si>
+  <si>
+    <t>BOX ABS 3.09X2.09X1.65" WHT</t>
+  </si>
+  <si>
+    <t>Q228-ND</t>
+  </si>
+  <si>
+    <t>739W-X2/03</t>
+  </si>
+  <si>
+    <t>OUTLET PWR NEMA 5-15R SNAPIN/IDC</t>
+  </si>
+  <si>
+    <t>6717 BK005-ND</t>
+  </si>
+  <si>
+    <t>6717 BK005</t>
+  </si>
+  <si>
+    <t>HOOK-UP STRND 14AWG BLACK 100'</t>
+  </si>
+  <si>
+    <t>6717 GR005-ND</t>
+  </si>
+  <si>
+    <t>6717 GR005</t>
+  </si>
+  <si>
+    <t>HOOK-UP STRND 14AWG GREEN 100'</t>
+  </si>
+  <si>
+    <t>6717 WH005-ND</t>
+  </si>
+  <si>
+    <t>6717 WH005</t>
+  </si>
+  <si>
+    <t>HOOK-UP STRND 14AWG WHITE 100'</t>
+  </si>
+  <si>
+    <t>#4 3/16" Panhead Self-Tapping Screws</t>
+  </si>
+  <si>
+    <t>92470a106</t>
+  </si>
+  <si>
+    <t>McMASTER-CARR</t>
+  </si>
+  <si>
+    <t>14AWG Black</t>
+  </si>
+  <si>
+    <t>14AWG Green</t>
+  </si>
+  <si>
+    <t>14AWG White</t>
+  </si>
+  <si>
+    <t>#4 Screw</t>
+  </si>
+  <si>
+    <t>ENCLOSURE</t>
+  </si>
+  <si>
+    <t>SOCKET</t>
   </si>
 </sst>
 </file>
@@ -862,7 +944,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -882,8 +964,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -891,8 +1009,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -902,6 +1025,24 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -911,6 +1052,24 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1244,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1261,9 +1420,10 @@
     <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1294,8 +1454,11 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1318,7 +1481,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1341,7 +1504,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1364,7 +1527,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1387,7 +1550,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1410,7 +1573,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1433,7 +1596,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1456,7 +1619,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1479,7 +1642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1502,7 +1665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1525,7 +1688,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1548,7 +1711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1571,7 +1734,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1594,7 +1757,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1617,7 +1780,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2361,7 +2524,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>1</v>
       </c>
@@ -2384,7 +2547,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>1</v>
       </c>
@@ -2410,7 +2573,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>1</v>
       </c>
@@ -2439,7 +2602,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2462,7 +2625,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>1</v>
       </c>
@@ -2485,7 +2648,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>1</v>
       </c>
@@ -2511,7 +2674,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:11">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2537,7 +2700,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:11">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2560,7 +2723,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:11">
       <c r="A57">
         <v>1</v>
       </c>
@@ -2581,6 +2744,130 @@
       </c>
       <c r="G57" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>264</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>265</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>260</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>261</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" t="s">
+        <v>256</v>
+      </c>
+      <c r="G63" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="F64" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K64" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2595,4 +2882,579 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>204</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>198</v>
+      </c>
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>